<commit_message>
running meridian for the first time
</commit_message>
<xml_diff>
--- a/Meridian/temp.xlsx
+++ b/Meridian/temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/ericjs_yu_mail_utoronto_ca/Documents/Desktop/LiquidIV/Meridian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_79C963C49B53948F6E38F4F7495DCE3A874432D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B3F8017-AE8E-4038-B6EA-242A6C0BB85D}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_79C963C49B53948F6E38F4F7495DCE3A874432D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CEF34F-0C89-4CF2-87EA-60B2FCBB73B0}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,9 +245,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -297,14 +294,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,12 +612,12 @@
   <dimension ref="A1:BU63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.765625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.23046875" bestFit="1" customWidth="1"/>
@@ -691,7 +689,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>